<commit_message>
updating to display unmet hours
</commit_message>
<xml_diff>
--- a/projects/dfg_temp.xlsx
+++ b/projects/dfg_temp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="780" windowWidth="14880" windowHeight="7365" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="780" windowWidth="14880" windowHeight="7365" tabRatio="562" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -2194,15 +2194,6 @@
     <t>standard_report_legacy.refrigeration_electricity</t>
   </si>
   <si>
-    <t>standard_reports.time_setpoint_not_met_during_occupied_cooling</t>
-  </si>
-  <si>
-    <t>standard_reports.time_setpoint_not_met_during_occupied_heating</t>
-  </si>
-  <si>
-    <t>standard_reports.time_setpoint_not_met_during_occupied_hours</t>
-  </si>
-  <si>
     <t>standard_reports.total_building_area</t>
   </si>
   <si>
@@ -2651,6 +2642,15 @@
   </si>
   <si>
     <t>discrete_uncertain</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.heating_hours_unmet</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.cooling_hours_unmet</t>
+  </si>
+  <si>
+    <t>standard_report_legacy.totals_hours_unmet</t>
   </si>
 </sst>
 </file>
@@ -6919,7 +6919,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -7012,7 +7012,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>664</v>
@@ -7240,7 +7240,7 @@
         <v>651</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7263,10 +7263,10 @@
         <v>652</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7299,9 +7299,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7504,7 +7504,7 @@
         <v>104</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7512,13 +7512,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E7" s="37" t="s">
         <v>68</v>
@@ -7531,16 +7531,16 @@
         <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="F8" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -7556,10 +7556,10 @@
         <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="F9" s="31" t="s">
         <v>619</v>
@@ -7579,10 +7579,10 @@
         <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="F10" s="31" t="s">
         <v>621</v>
@@ -7597,35 +7597,35 @@
         <v>22</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="I11" s="31"/>
       <c r="J11" s="31" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="K11" s="31" t="s">
+        <v>862</v>
+      </c>
+      <c r="L11" s="31" t="s">
+        <v>864</v>
+      </c>
+      <c r="M11" s="31" t="s">
+        <v>864</v>
+      </c>
+      <c r="O11" s="31" t="s">
         <v>865</v>
       </c>
-      <c r="L11" s="31" t="s">
-        <v>867</v>
-      </c>
-      <c r="M11" s="31" t="s">
-        <v>867</v>
-      </c>
-      <c r="O11" s="31" t="s">
-        <v>868</v>
-      </c>
       <c r="Q11" s="52" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
     </row>
     <row r="12" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -7633,13 +7633,13 @@
         <v>0</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>68</v>
@@ -7652,16 +7652,16 @@
         <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="F13" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -7677,10 +7677,10 @@
         <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>619</v>
@@ -7700,10 +7700,10 @@
         <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="F15" s="31" t="s">
         <v>621</v>
@@ -7718,16 +7718,16 @@
         <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="I16" s="31"/>
     </row>
@@ -7736,13 +7736,13 @@
         <v>0</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E17" s="37" t="s">
         <v>68</v>
@@ -7755,16 +7755,16 @@
         <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -7780,10 +7780,10 @@
         <v>21</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>619</v>
@@ -7803,10 +7803,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="F20" s="31" t="s">
         <v>621</v>
@@ -7821,16 +7821,16 @@
         <v>21</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="I21" s="31"/>
     </row>
@@ -7839,13 +7839,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="E22" s="37" t="s">
         <v>68</v>
@@ -7858,10 +7858,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="F23" s="31" t="s">
         <v>630</v>
@@ -7883,10 +7883,10 @@
         <v>21</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>619</v>
@@ -7909,10 +7909,10 @@
         <v>21</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>619</v>
@@ -7930,10 +7930,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>619</v>
@@ -7948,13 +7948,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="E27" s="49" t="s">
         <v>68</v>
@@ -7986,13 +7986,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="E29" s="37" t="s">
         <v>68</v>
@@ -8005,10 +8005,10 @@
         <v>21</v>
       </c>
       <c r="D30" s="46" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="E30" s="46" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="F30" s="31" t="s">
         <v>619</v>
@@ -8023,10 +8023,10 @@
         <v>21</v>
       </c>
       <c r="D31" s="46" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="E31" s="46" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="F31" s="31" t="s">
         <v>619</v>
@@ -8041,13 +8041,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="E32" s="37" t="s">
         <v>68</v>
@@ -8060,10 +8060,10 @@
         <v>21</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="F33" s="31" t="s">
         <v>619</v>
@@ -8085,13 +8085,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="E34" s="37" t="s">
         <v>68</v>
@@ -8104,10 +8104,10 @@
         <v>21</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="F35" s="31" t="s">
         <v>619</v>
@@ -8129,13 +8129,13 @@
         <v>1</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="E36" s="37" t="s">
         <v>68</v>
@@ -8148,10 +8148,10 @@
         <v>21</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>619</v>
@@ -8173,13 +8173,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="47" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="D38" s="47" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="E38" s="47" t="s">
         <v>68</v>
@@ -8192,13 +8192,13 @@
         <v>1</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="E39" s="37" t="s">
         <v>68</v>
@@ -8211,13 +8211,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D40" s="37" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="E40" s="37" t="s">
         <v>68</v>
@@ -8230,10 +8230,10 @@
         <v>21</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="F41" s="31" t="s">
         <v>619</v>
@@ -8255,13 +8255,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="D42" s="37" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="E42" s="37" t="s">
         <v>68</v>
@@ -8302,7 +8302,7 @@
         <v>619</v>
       </c>
       <c r="G44" s="31" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="H44" s="31">
         <v>0</v>
@@ -8321,13 +8321,13 @@
         <v>1</v>
       </c>
       <c r="B45" s="47" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="C45" s="47" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="D45" s="47" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="E45" s="47" t="s">
         <v>68</v>
@@ -8340,10 +8340,10 @@
         <v>21</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>619</v>
@@ -8365,13 +8365,13 @@
         <v>1</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="D47" s="37" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="E47" s="37" t="s">
         <v>68</v>
@@ -8384,10 +8384,10 @@
         <v>21</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="E48" s="31" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="F48" s="31" t="s">
         <v>619</v>
@@ -8409,13 +8409,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="D49" s="37" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="E49" s="37" t="s">
         <v>68</v>
@@ -8428,10 +8428,10 @@
         <v>21</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E50" s="31" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="F50" s="31" t="s">
         <v>619</v>
@@ -8453,13 +8453,13 @@
         <v>1</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="C51" s="37" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D51" s="37" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="E51" s="37" t="s">
         <v>68</v>
@@ -8472,10 +8472,10 @@
         <v>21</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="F52" s="31" t="s">
         <v>619</v>
@@ -8497,13 +8497,13 @@
         <v>1</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C53" s="37" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D53" s="37" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="E53" s="37" t="s">
         <v>68</v>
@@ -8516,10 +8516,10 @@
         <v>21</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="E54" s="31" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="F54" s="31" t="s">
         <v>619</v>
@@ -8541,13 +8541,13 @@
         <v>1</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C55" s="37" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="D55" s="37" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="E55" s="37" t="s">
         <v>68</v>
@@ -8560,10 +8560,10 @@
         <v>21</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>619</v>
@@ -8585,13 +8585,13 @@
         <v>1</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C57" s="37" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="D57" s="37" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="E57" s="37" t="s">
         <v>68</v>
@@ -8604,10 +8604,10 @@
         <v>21</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="E58" s="31" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="F58" s="31" t="s">
         <v>619</v>
@@ -8629,13 +8629,13 @@
         <v>1</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="C59" s="37" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="D59" s="37" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="E59" s="37" t="s">
         <v>68</v>
@@ -8648,10 +8648,10 @@
         <v>21</v>
       </c>
       <c r="D60" s="31" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="E60" s="31" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="F60" s="31" t="s">
         <v>619</v>
@@ -8673,10 +8673,10 @@
         <v>21</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="E61" s="31" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="F61" s="31" t="s">
         <v>619</v>
@@ -8698,13 +8698,13 @@
         <v>1</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="D62" s="37" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="E62" s="37" t="s">
         <v>68</v>
@@ -8717,13 +8717,13 @@
         <v>1</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>68</v>
@@ -8736,13 +8736,13 @@
         <v>1</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -8755,13 +8755,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="D65" s="37" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="E65" s="37" t="s">
         <v>68</v>
@@ -8774,13 +8774,13 @@
         <v>1</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -8793,13 +8793,13 @@
         <v>1</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>
@@ -8812,13 +8812,13 @@
         <v>1</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="D68" s="37" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>68</v>
@@ -8831,13 +8831,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="37" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="C69" s="37" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="D69" s="37" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="E69" s="37" t="s">
         <v>68</v>
@@ -8850,13 +8850,13 @@
         <v>1</v>
       </c>
       <c r="B70" s="37" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="C70" s="37" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="D70" s="37" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="E70" s="37" t="s">
         <v>68</v>
@@ -9103,9 +9103,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22:C25"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9727,7 +9727,7 @@
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40" t="s">
-        <v>717</v>
+        <v>868</v>
       </c>
       <c r="D22" s="40" t="s">
         <v>684</v>
@@ -9736,7 +9736,7 @@
         <v>64</v>
       </c>
       <c r="F22" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="40" t="b">
         <v>1</v>
@@ -9755,7 +9755,7 @@
       </c>
       <c r="B23" s="40"/>
       <c r="C23" s="40" t="s">
-        <v>718</v>
+        <v>867</v>
       </c>
       <c r="D23" s="40" t="s">
         <v>684</v>
@@ -9764,7 +9764,7 @@
         <v>64</v>
       </c>
       <c r="F23" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="40" t="b">
         <v>1</v>
@@ -9783,7 +9783,7 @@
       </c>
       <c r="B24" s="40"/>
       <c r="C24" s="40" t="s">
-        <v>719</v>
+        <v>869</v>
       </c>
       <c r="D24" s="40" t="s">
         <v>684</v>
@@ -9792,7 +9792,7 @@
         <v>64</v>
       </c>
       <c r="F24" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="40" t="b">
         <v>1</v>
@@ -9811,7 +9811,7 @@
       </c>
       <c r="B25" s="40"/>
       <c r="C25" s="40" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="D25" s="40" t="s">
         <v>688</v>

</xml_diff>

<commit_message>
minor updates to m0
I also made updates to my test spreadsheet to quickly run a variety of
system combinations.
</commit_message>
<xml_diff>
--- a/projects/dfg_temp.xlsx
+++ b/projects/dfg_temp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="780" windowWidth="14880" windowHeight="7365" tabRatio="562" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="780" windowWidth="14880" windowHeight="7365" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2434" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2450" uniqueCount="873">
   <si>
     <t>type</t>
   </si>
@@ -2509,9 +2509,6 @@
     <t>Add Interior Constructions to Adiabatic Surfaces</t>
   </si>
   <si>
-    <t>HVAC System Type</t>
-  </si>
-  <si>
     <t>hvac_system_type</t>
   </si>
   <si>
@@ -2651,6 +2648,18 @@
   </si>
   <si>
     <t>standard_report_legacy.totals_hours_unmet</t>
+  </si>
+  <si>
+    <t>HVAC System Type-a</t>
+  </si>
+  <si>
+    <t>HVAC System Type-b</t>
+  </si>
+  <si>
+    <t>HVAC System Type-c</t>
+  </si>
+  <si>
+    <t>|"SysType 1","SysType 2","SysType 3","SysType 4","SysType 5","SysType 6","SysType 7","SysType 8"|</t>
   </si>
 </sst>
 </file>
@@ -6860,8 +6869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6919,7 +6928,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -7126,17 +7135,20 @@
         <v>570</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="34"/>
+      <c r="G24" s="30" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="30">
-        <v>8</v>
+        <v>1024</v>
       </c>
       <c r="C25" s="33"/>
       <c r="D25" s="34"/>
@@ -7240,7 +7252,7 @@
         <v>651</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7299,9 +7311,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y125"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7565,7 +7577,7 @@
         <v>619</v>
       </c>
       <c r="H9" s="4">
-        <v>1</v>
+        <v>0.873</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -7597,40 +7609,42 @@
         <v>22</v>
       </c>
       <c r="D11" s="31" t="s">
+        <v>869</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>822</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>823</v>
       </c>
       <c r="F11" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>857</v>
-      </c>
-      <c r="I11" s="31"/>
+        <v>856</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>872</v>
+      </c>
       <c r="J11" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>861</v>
+      </c>
+      <c r="L11" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="M11" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="O11" s="31" t="s">
         <v>864</v>
       </c>
-      <c r="K11" s="31" t="s">
-        <v>862</v>
-      </c>
-      <c r="L11" s="31" t="s">
-        <v>864</v>
-      </c>
-      <c r="M11" s="31" t="s">
-        <v>864</v>
-      </c>
-      <c r="O11" s="31" t="s">
+      <c r="Q11" s="52" t="s">
         <v>865</v>
-      </c>
-      <c r="Q11" s="52" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="12" spans="1:25" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" s="37" t="s">
         <v>793</v>
@@ -7715,25 +7729,45 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="31" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="31" t="s">
+        <v>870</v>
+      </c>
+      <c r="E16" s="31" t="s">
         <v>822</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>823</v>
       </c>
       <c r="F16" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>857</v>
-      </c>
-      <c r="I16" s="31"/>
+        <v>856</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>872</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="K16" s="31" t="s">
+        <v>861</v>
+      </c>
+      <c r="L16" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="M16" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="O16" s="31" t="s">
+        <v>864</v>
+      </c>
+      <c r="Q16" s="52" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="17" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>794</v>
@@ -7818,21 +7852,41 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" s="31" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21" s="31" t="s">
+        <v>871</v>
+      </c>
+      <c r="E21" s="31" t="s">
         <v>822</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>823</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>857</v>
-      </c>
-      <c r="I21" s="31"/>
+        <v>856</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>872</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="K21" s="31" t="s">
+        <v>861</v>
+      </c>
+      <c r="L21" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="M21" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="O21" s="31" t="s">
+        <v>864</v>
+      </c>
+      <c r="Q21" s="52" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="22" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="b">
@@ -7945,16 +7999,16 @@
     </row>
     <row r="27" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>858</v>
+        <v>332</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>859</v>
+        <v>333</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>863</v>
+        <v>333</v>
       </c>
       <c r="E27" s="49" t="s">
         <v>68</v>
@@ -7964,16 +8018,16 @@
     </row>
     <row r="28" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>332</v>
+        <v>857</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>333</v>
+        <v>858</v>
       </c>
       <c r="D28" s="49" t="s">
-        <v>333</v>
+        <v>862</v>
       </c>
       <c r="E28" s="49" t="s">
         <v>68</v>
@@ -7986,13 +8040,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="37" t="s">
+        <v>852</v>
+      </c>
+      <c r="C29" s="37" t="s">
         <v>853</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="D29" s="37" t="s">
         <v>854</v>
-      </c>
-      <c r="D29" s="37" t="s">
-        <v>855</v>
       </c>
       <c r="E29" s="37" t="s">
         <v>68</v>
@@ -8258,7 +8312,7 @@
         <v>772</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D42" s="37" t="s">
         <v>746</v>
@@ -8340,10 +8394,10 @@
         <v>21</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>619</v>
@@ -8698,13 +8752,13 @@
         <v>1</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C62" s="37" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D62" s="37" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E62" s="37" t="s">
         <v>68</v>
@@ -8717,13 +8771,13 @@
         <v>1</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C63" s="37" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E63" s="37" t="s">
         <v>68</v>
@@ -8736,13 +8790,13 @@
         <v>1</v>
       </c>
       <c r="B64" s="37" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C64" s="37" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D64" s="37" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E64" s="37" t="s">
         <v>68</v>
@@ -8755,13 +8809,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="37" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C65" s="37" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D65" s="37" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E65" s="37" t="s">
         <v>68</v>
@@ -8774,13 +8828,13 @@
         <v>1</v>
       </c>
       <c r="B66" s="37" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D66" s="37" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E66" s="37" t="s">
         <v>68</v>
@@ -8793,13 +8847,13 @@
         <v>1</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D67" s="37" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>68</v>
@@ -8812,13 +8866,13 @@
         <v>1</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D68" s="37" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>68</v>
@@ -8831,13 +8885,13 @@
         <v>1</v>
       </c>
       <c r="B69" s="37" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C69" s="37" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D69" s="37" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E69" s="37" t="s">
         <v>68</v>
@@ -8850,13 +8904,13 @@
         <v>1</v>
       </c>
       <c r="B70" s="37" t="s">
+        <v>823</v>
+      </c>
+      <c r="C70" s="37" t="s">
         <v>824</v>
       </c>
-      <c r="C70" s="37" t="s">
+      <c r="D70" s="37" t="s">
         <v>825</v>
-      </c>
-      <c r="D70" s="37" t="s">
-        <v>826</v>
       </c>
       <c r="E70" s="37" t="s">
         <v>68</v>
@@ -9103,9 +9157,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9727,7 +9781,7 @@
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D22" s="40" t="s">
         <v>684</v>
@@ -9755,7 +9809,7 @@
       </c>
       <c r="B23" s="40"/>
       <c r="C23" s="40" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D23" s="40" t="s">
         <v>684</v>
@@ -9783,7 +9837,7 @@
       </c>
       <c r="B24" s="40"/>
       <c r="C24" s="40" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D24" s="40" t="s">
         <v>684</v>
@@ -9910,7 +9964,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" s="40">
         <v>0</v>
@@ -9940,7 +9994,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" s="40">
         <v>0</v>
@@ -9970,7 +10024,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" s="40">
         <v>0</v>
@@ -10000,7 +10054,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" s="40">
         <v>0</v>
@@ -18253,7 +18307,7 @@
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="F17:G18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update to hvac test workflow
</commit_message>
<xml_diff>
--- a/projects/dfg_temp.xlsx
+++ b/projects/dfg_temp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="780" windowWidth="14880" windowHeight="7365" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="780" windowWidth="14880" windowHeight="7365" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2450" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="876">
   <si>
     <t>type</t>
   </si>
@@ -2660,6 +2660,15 @@
   </si>
   <si>
     <t>|"SysType 1","SysType 2","SysType 3","SysType 4","SysType 5","SysType 6","SysType 7","SysType 8"|</t>
+  </si>
+  <si>
+    <t>COFFEE Annual Summary Report</t>
+  </si>
+  <si>
+    <t>coffee_annual_summary_report</t>
+  </si>
+  <si>
+    <t>COFFEEAnnualSummaryReport</t>
   </si>
 </sst>
 </file>
@@ -4728,10 +4737,10 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1801">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6869,7 +6878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -7311,9 +7320,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y125"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7367,14 +7376,14 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="51" t="s">
+      <c r="T1" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
     </row>
     <row r="2" spans="1:25" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -7638,7 +7647,7 @@
       <c r="O11" s="31" t="s">
         <v>864</v>
       </c>
-      <c r="Q11" s="52" t="s">
+      <c r="Q11" s="51" t="s">
         <v>865</v>
       </c>
     </row>
@@ -7761,7 +7770,7 @@
       <c r="O16" s="31" t="s">
         <v>864</v>
       </c>
-      <c r="Q16" s="52" t="s">
+      <c r="Q16" s="51" t="s">
         <v>865</v>
       </c>
     </row>
@@ -7884,7 +7893,7 @@
       <c r="O21" s="31" t="s">
         <v>864</v>
       </c>
-      <c r="Q21" s="52" t="s">
+      <c r="Q21" s="51" t="s">
         <v>865</v>
       </c>
     </row>
@@ -8918,9 +8927,24 @@
       <c r="G70" s="38"/>
       <c r="H70" s="38"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H71" s="31"/>
-      <c r="I71" s="31"/>
+    <row r="71" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="B71" s="37" t="s">
+        <v>873</v>
+      </c>
+      <c r="C71" s="37" t="s">
+        <v>874</v>
+      </c>
+      <c r="D71" s="37" t="s">
+        <v>875</v>
+      </c>
+      <c r="E71" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H72" s="31"/>

</xml_diff>